<commit_message>
Update intial_data.xlsx to have year campaigns
</commit_message>
<xml_diff>
--- a/migration_data/initial_data.xlsx
+++ b/migration_data/initial_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/Dropbox/vhosts/clients/rhizome/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/Dropbox/vhosts/clients/rhizome/migration_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -42957,11 +42957,11 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">NOW()</f>
-        <v>42487.817650694444</v>
+        <v>42506.724766319443</v>
       </c>
       <c r="C2" s="14">
         <f ca="1">NOW()</f>
-        <v>42487.817650694444</v>
+        <v>42506.724766319443</v>
       </c>
       <c r="D2" t="s">
         <v>1054</v>
@@ -42973,11 +42973,11 @@
       </c>
       <c r="B3" s="14">
         <f ca="1">NOW()</f>
-        <v>42487.817650694444</v>
+        <v>42506.724766319443</v>
       </c>
       <c r="C3" s="14">
         <f ca="1">NOW()</f>
-        <v>42487.817650694444</v>
+        <v>42506.724766319443</v>
       </c>
       <c r="D3" t="s">
         <v>1054</v>
@@ -81423,10 +81423,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -81615,6 +81615,110 @@
         <v>1</v>
       </c>
       <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>2014</v>
+      </c>
+      <c r="B8" s="12">
+        <v>41640</v>
+      </c>
+      <c r="C8" s="12">
+        <v>42004</v>
+      </c>
+      <c r="D8">
+        <v>2014</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>2015</v>
+      </c>
+      <c r="B9" s="12">
+        <v>42005</v>
+      </c>
+      <c r="C9" s="12">
+        <v>42369</v>
+      </c>
+      <c r="D9">
+        <v>2015</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>2016</v>
+      </c>
+      <c r="B10" s="12">
+        <v>42370</v>
+      </c>
+      <c r="C10" s="12">
+        <v>42735</v>
+      </c>
+      <c r="D10">
+        <v>2016</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11">
+        <v>2017</v>
+      </c>
+      <c r="B11" s="12">
+        <v>42736</v>
+      </c>
+      <c r="C11" s="12">
+        <v>43100</v>
+      </c>
+      <c r="D11">
+        <v>2017</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cleanup migration histoy and add more docker instructions for development
</commit_message>
<xml_diff>
--- a/migration_data/initial_data.xlsx
+++ b/migration_data/initial_data.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26101"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dima/Dropbox/vhosts/clients/rhizome/migration_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/john/code/docker/rhizome/migration_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21060" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_tag" sheetId="1" r:id="rId1"/>
@@ -42957,11 +42957,11 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">NOW()</f>
-        <v>42506.724766319443</v>
+        <v>42579.420037037038</v>
       </c>
       <c r="C2" s="14">
         <f ca="1">NOW()</f>
-        <v>42506.724766319443</v>
+        <v>42579.420037037038</v>
       </c>
       <c r="D2" t="s">
         <v>1054</v>
@@ -42973,11 +42973,11 @@
       </c>
       <c r="B3" s="14">
         <f ca="1">NOW()</f>
-        <v>42506.724766319443</v>
+        <v>42579.420037037038</v>
       </c>
       <c r="C3" s="14">
         <f ca="1">NOW()</f>
-        <v>42506.724766319443</v>
+        <v>42579.420037037038</v>
       </c>
       <c r="D3" t="s">
         <v>1054</v>
@@ -81619,108 +81619,20 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8">
-        <v>2014</v>
-      </c>
-      <c r="B8" s="12">
-        <v>41640</v>
-      </c>
-      <c r="C8" s="12">
-        <v>42004</v>
-      </c>
-      <c r="D8">
-        <v>2014</v>
-      </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>1</v>
-      </c>
-      <c r="H8">
-        <v>1</v>
-      </c>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9">
-        <v>2015</v>
-      </c>
-      <c r="B9" s="12">
-        <v>42005</v>
-      </c>
-      <c r="C9" s="12">
-        <v>42369</v>
-      </c>
-      <c r="D9">
-        <v>2015</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>1</v>
-      </c>
-      <c r="H9">
-        <v>1</v>
-      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10">
-        <v>2016</v>
-      </c>
-      <c r="B10" s="12">
-        <v>42370</v>
-      </c>
-      <c r="C10" s="12">
-        <v>42735</v>
-      </c>
-      <c r="D10">
-        <v>2016</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-      <c r="H10">
-        <v>1</v>
-      </c>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11">
-        <v>2017</v>
-      </c>
-      <c r="B11" s="12">
-        <v>42736</v>
-      </c>
-      <c r="C11" s="12">
-        <v>43100</v>
-      </c>
-      <c r="D11">
-        <v>2017</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11">
-        <v>1</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
+      <c r="B11" s="12"/>
+      <c r="C11" s="12"/>
     </row>
   </sheetData>
   <sortState ref="B2:D15">

</xml_diff>

<commit_message>
add the file_type column only if it does not exist
</commit_message>
<xml_diff>
--- a/migration_data/initial_data.xlsx
+++ b/migration_data/initial_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="indicator_tag" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3622" uniqueCount="2306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3658" uniqueCount="2308">
   <si>
     <t>tag_name</t>
   </si>
@@ -6956,6 +6956,12 @@
   </si>
   <si>
     <t>November 2015 - OPV - LPD</t>
+  </si>
+  <si>
+    <t>resource_name</t>
+  </si>
+  <si>
+    <t>campaign</t>
   </si>
 </sst>
 </file>
@@ -7631,7 +7637,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8614"/>
   <sheetViews>
-    <sheetView topLeftCell="A496" zoomScale="106" workbookViewId="0">
+    <sheetView zoomScale="106" workbookViewId="0">
       <selection activeCell="C514" sqref="A2:C514"/>
     </sheetView>
   </sheetViews>
@@ -42957,11 +42963,11 @@
       </c>
       <c r="B2" s="14">
         <f ca="1">NOW()</f>
-        <v>42579.420037037038</v>
+        <v>42581.707936921295</v>
       </c>
       <c r="C2" s="14">
         <f ca="1">NOW()</f>
-        <v>42579.420037037038</v>
+        <v>42581.707936921295</v>
       </c>
       <c r="D2" t="s">
         <v>1054</v>
@@ -42973,11 +42979,11 @@
       </c>
       <c r="B3" s="14">
         <f ca="1">NOW()</f>
-        <v>42579.420037037038</v>
+        <v>42581.707936921295</v>
       </c>
       <c r="C3" s="14">
         <f ca="1">NOW()</f>
-        <v>42579.420037037038</v>
+        <v>42581.707936921295</v>
       </c>
       <c r="D3" t="s">
         <v>1054</v>
@@ -45016,8 +45022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -45028,7 +45034,7 @@
     <col min="8" max="8" width="22.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>5</v>
       </c>
@@ -45053,8 +45059,11 @@
       <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I1" s="1" t="s">
+        <v>2306</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -45079,8 +45088,11 @@
       <c r="H2" s="6" t="s">
         <v>1060</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I2" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -45105,8 +45117,11 @@
       <c r="H3" s="6" t="s">
         <v>1060</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I3" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -45131,8 +45146,11 @@
       <c r="H4" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I4" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -45157,8 +45175,11 @@
       <c r="H5" s="3" t="s">
         <v>1059</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I5" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -45183,8 +45204,11 @@
       <c r="H6" s="3" t="s">
         <v>1060</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I6" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -45209,8 +45233,11 @@
       <c r="H7" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I7" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -45235,8 +45262,11 @@
       <c r="H8" s="6" t="s">
         <v>1060</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I8" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -45261,8 +45291,11 @@
       <c r="H9" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I9" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -45287,8 +45320,11 @@
       <c r="H10" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I10" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -45313,8 +45349,11 @@
       <c r="H11" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I11" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -45339,8 +45378,11 @@
       <c r="H12" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I12" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -45365,8 +45407,11 @@
       <c r="H13" s="3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I13" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -45391,8 +45436,11 @@
       <c r="H14" s="3" t="s">
         <v>1063</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I14" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -45417,8 +45465,11 @@
       <c r="H15" s="3" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="I15" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -45442,6 +45493,9 @@
       </c>
       <c r="H16" s="3" t="s">
         <v>44</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>2307</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="16" x14ac:dyDescent="0.2">
@@ -45469,6 +45523,9 @@
       <c r="H17" s="3" t="s">
         <v>50</v>
       </c>
+      <c r="I17" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="18" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
@@ -45495,6 +45552,9 @@
       <c r="H18" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="I18" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="19" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
@@ -45521,6 +45581,9 @@
       <c r="H19" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="I19" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="20" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
@@ -45547,6 +45610,9 @@
       <c r="H20" s="3" t="s">
         <v>18</v>
       </c>
+      <c r="I20" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="21" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
@@ -45573,6 +45639,9 @@
       <c r="H21" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="I21" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="22" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
@@ -45599,6 +45668,9 @@
       <c r="H22" s="3" t="s">
         <v>2258</v>
       </c>
+      <c r="I22" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="23" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
@@ -45625,6 +45697,9 @@
       <c r="H23" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="I23" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="24" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
@@ -45651,6 +45726,9 @@
       <c r="H24" s="3" t="s">
         <v>51</v>
       </c>
+      <c r="I24" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="25" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
@@ -45677,6 +45755,9 @@
       <c r="H25" s="3" t="s">
         <v>33</v>
       </c>
+      <c r="I25" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="26" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
@@ -45703,6 +45784,9 @@
       <c r="H26" s="3" t="s">
         <v>1060</v>
       </c>
+      <c r="I26" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="27" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
@@ -45729,6 +45813,9 @@
       <c r="H27" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="I27" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="28" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="10">
@@ -45755,6 +45842,9 @@
       <c r="H28" s="6" t="s">
         <v>1060</v>
       </c>
+      <c r="I28" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="29" spans="1:19" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="6">
@@ -45781,7 +45871,9 @@
       <c r="H29" s="6" t="s">
         <v>1060</v>
       </c>
-      <c r="I29" s="4"/>
+      <c r="I29" s="6" t="s">
+        <v>2307</v>
+      </c>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
       <c r="L29" s="4"/>
@@ -45818,7 +45910,9 @@
       <c r="H30" s="6" t="s">
         <v>1060</v>
       </c>
-      <c r="I30" s="6"/>
+      <c r="I30" s="6" t="s">
+        <v>2307</v>
+      </c>
       <c r="J30" s="6"/>
       <c r="K30" s="6"/>
       <c r="L30" s="6"/>
@@ -45855,6 +45949,9 @@
       <c r="H31" s="6" t="s">
         <v>50</v>
       </c>
+      <c r="I31" s="6" t="s">
+        <v>2307</v>
+      </c>
     </row>
     <row r="32" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -45881,8 +45978,11 @@
       <c r="H32" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I32" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -45907,8 +46007,11 @@
       <c r="H33" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I33" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -45933,8 +46036,11 @@
       <c r="H34" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I34" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -45959,8 +46065,11 @@
       <c r="H35" s="6" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I35" s="6" t="s">
+        <v>2307</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -45984,6 +46093,9 @@
       </c>
       <c r="H36" s="6" t="s">
         <v>1060</v>
+      </c>
+      <c r="I36" s="6" t="s">
+        <v>2307</v>
       </c>
     </row>
   </sheetData>
@@ -81425,8 +81537,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>